<commit_message>
Add support for uploading Excel files to the analytics dashboard
Remove debug logging from CSV parsing and XLSX conversion, and update documentation to reflect XLSX support.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 249a40c3-8898-4ba6-a12c-64e84a5be732
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/68e0c2b3-7367-4833-8a0d-e371ebee37a6/249a40c3-8898-4ba6-a12c-64e84a5be732/VENjD8q
</commit_message>
<xml_diff>
--- a/public/sample-clearent.xlsx
+++ b/public/sample-clearent.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -980,14 +980,9 @@
         <v>2024-03</v>
       </c>
     </row>
-    <row r="35">
-      <c r="A35" t="str">
-        <v/>
-      </c>
-    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E35"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E34"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>